<commit_message>
updating melting point data adding melting point in kelvin
</commit_message>
<xml_diff>
--- a/Machine learning/docs/Pubchem_melting_dataset_fromXML.xlsx
+++ b/Machine learning/docs/Pubchem_melting_dataset_fromXML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\BIOINFORMAICS\Machine Learning\Machine learning\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3A3B690-EB9E-435A-A79B-AFA91698F1A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7EFF0C-D7BB-4505-9A1C-BF77BF1891E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{824F0F9F-75C4-40E3-AD7C-0727C9042DB4}"/>
   </bookViews>
@@ -7741,11 +7741,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="20% - Accent3" xfId="1" builtinId="38"/>
@@ -56897,13 +56897,14 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="14" style="4" customWidth="1"/>
+    <col min="2" max="2" width="14" style="4" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" customWidth="1"/>
     <col min="4" max="4" width="19.44140625" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
     <col min="9" max="9" width="33.44140625" customWidth="1"/>
@@ -56917,7 +56918,7 @@
       <c r="B1" s="3" t="s">
         <v>2522</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2525</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -56926,10 +56927,10 @@
       <c r="E1" s="2" t="s">
         <v>2523</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="7" t="s">
         <v>2527</v>
       </c>
-      <c r="J1" s="5"/>
+      <c r="J1" s="7"/>
     </row>
     <row r="2" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -56938,11 +56939,14 @@
       <c r="B2" s="4">
         <v>135</v>
       </c>
+      <c r="C2">
+        <v>408.15</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="7"/>
     </row>
     <row r="3" spans="1:10" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -56951,11 +56955,14 @@
       <c r="B3" s="4">
         <v>58</v>
       </c>
+      <c r="C3">
+        <v>331.15</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="7"/>
     </row>
     <row r="4" spans="1:10" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -56964,13 +56971,16 @@
       <c r="B4" s="4">
         <v>61</v>
       </c>
+      <c r="C4">
+        <v>334.15</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="5" t="s">
         <v>2526</v>
       </c>
-      <c r="J4" s="7"/>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
@@ -56979,11 +56989,14 @@
       <c r="B5" s="4">
         <v>67</v>
       </c>
+      <c r="C5">
+        <v>340.15</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -56992,6 +57005,9 @@
       <c r="B6" s="4">
         <v>71</v>
       </c>
+      <c r="C6">
+        <v>344.15</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>56</v>
       </c>
@@ -57008,6 +57024,9 @@
         <f>MEDIAN(150,155)</f>
         <v>152.5</v>
       </c>
+      <c r="C7">
+        <v>425.65</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>57</v>
       </c>
@@ -57022,6 +57041,9 @@
         <f>AVERAGE(61, 55, 61, 55, 55)</f>
         <v>57.4</v>
       </c>
+      <c r="C8">
+        <v>330.55</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>58</v>
       </c>
@@ -57033,6 +57055,9 @@
       <c r="B9" s="4">
         <v>60</v>
       </c>
+      <c r="C9">
+        <v>333.15</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>59</v>
       </c>
@@ -57044,6 +57069,9 @@
       <c r="B10" s="4">
         <v>61</v>
       </c>
+      <c r="C10">
+        <v>334.15</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>60</v>
       </c>
@@ -57055,6 +57083,9 @@
       <c r="B11" s="4">
         <v>53</v>
       </c>
+      <c r="C11">
+        <v>326.14999999999998</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>61</v>
       </c>
@@ -57067,6 +57098,9 @@
       <c r="B12" s="4">
         <v>76</v>
       </c>
+      <c r="C12">
+        <v>349.15</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>62</v>
       </c>
@@ -57078,6 +57112,9 @@
       <c r="B13" s="4">
         <v>60</v>
       </c>
+      <c r="C13">
+        <v>333.15</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>63</v>
       </c>
@@ -57089,6 +57126,9 @@
       <c r="B14" s="4">
         <v>53</v>
       </c>
+      <c r="C14">
+        <v>326.14999999999998</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>64</v>
       </c>
@@ -57100,6 +57140,9 @@
       <c r="B15" s="4">
         <v>61</v>
       </c>
+      <c r="C15">
+        <v>334.15</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>65</v>
       </c>
@@ -57112,6 +57155,9 @@
         <f>MEDIAN(2,8)</f>
         <v>5</v>
       </c>
+      <c r="C16">
+        <v>278.14999999999998</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>66</v>
       </c>
@@ -57123,6 +57169,9 @@
       <c r="B17" s="4">
         <v>57</v>
       </c>
+      <c r="C17">
+        <v>330.15</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>67</v>
       </c>
@@ -57134,6 +57183,9 @@
       <c r="B18" s="4">
         <v>55</v>
       </c>
+      <c r="C18">
+        <v>328.15</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>68</v>
       </c>
@@ -57146,6 +57198,9 @@
         <f>MEDIAN(229,230)</f>
         <v>229.5</v>
       </c>
+      <c r="C19">
+        <v>502.65</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>69</v>
       </c>
@@ -57157,6 +57212,9 @@
       <c r="B20" s="4">
         <v>70</v>
       </c>
+      <c r="C20">
+        <v>343.15</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>70</v>
       </c>
@@ -57168,6 +57226,9 @@
       <c r="B21" s="4">
         <v>60</v>
       </c>
+      <c r="C21">
+        <v>333.15</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>71</v>
       </c>
@@ -57179,6 +57240,9 @@
       <c r="B22" s="4">
         <v>81</v>
       </c>
+      <c r="C22">
+        <v>354.15</v>
+      </c>
       <c r="E22" s="1" t="s">
         <v>72</v>
       </c>
@@ -57190,6 +57254,9 @@
       <c r="B23" s="4">
         <v>60</v>
       </c>
+      <c r="C23">
+        <v>333.15</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>73</v>
       </c>
@@ -57201,6 +57268,9 @@
       <c r="B24" s="4">
         <v>55</v>
       </c>
+      <c r="C24">
+        <v>328.15</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>74</v>
       </c>
@@ -57212,6 +57282,9 @@
       <c r="B25" s="4">
         <v>61</v>
       </c>
+      <c r="C25">
+        <v>334.15</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>75</v>
       </c>
@@ -57223,6 +57296,9 @@
       <c r="B26" s="4">
         <v>58</v>
       </c>
+      <c r="C26">
+        <v>331.15</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>76</v>
       </c>
@@ -57234,6 +57310,9 @@
       <c r="B27" s="4">
         <v>61</v>
       </c>
+      <c r="C27">
+        <v>334.15</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>77</v>
       </c>
@@ -57245,6 +57324,9 @@
       <c r="B28" s="4">
         <v>55</v>
       </c>
+      <c r="C28">
+        <v>328.15</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>78</v>
       </c>
@@ -57256,6 +57338,9 @@
       <c r="B29" s="4">
         <v>81</v>
       </c>
+      <c r="C29">
+        <v>354.15</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>79</v>
       </c>
@@ -57267,6 +57352,9 @@
       <c r="B30" s="4">
         <v>81</v>
       </c>
+      <c r="C30">
+        <v>354.15</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>80</v>
       </c>
@@ -57279,6 +57367,9 @@
         <f>MEDIAN(49,54)</f>
         <v>51.5</v>
       </c>
+      <c r="C31">
+        <v>324.64999999999998</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>81</v>
       </c>
@@ -57290,6 +57381,9 @@
       <c r="B32" s="4">
         <v>76</v>
       </c>
+      <c r="C32">
+        <v>349.15</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>82</v>
       </c>
@@ -57301,6 +57395,9 @@
       <c r="B33" s="4">
         <v>61</v>
       </c>
+      <c r="C33">
+        <v>334.15</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>83</v>
       </c>
@@ -57312,6 +57409,9 @@
       <c r="B34" s="4">
         <v>61</v>
       </c>
+      <c r="C34">
+        <v>334.15</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>84</v>
       </c>
@@ -57323,6 +57423,9 @@
       <c r="B35" s="4">
         <v>61</v>
       </c>
+      <c r="C35">
+        <v>334.15</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>85</v>
       </c>
@@ -57335,6 +57438,9 @@
         <f>MEDIAN(50,60)</f>
         <v>55</v>
       </c>
+      <c r="C36">
+        <v>328.15</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>86</v>
       </c>
@@ -57346,6 +57452,9 @@
       <c r="B37" s="4">
         <v>61</v>
       </c>
+      <c r="C37">
+        <v>334.15</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>87</v>
       </c>
@@ -57357,6 +57466,9 @@
       <c r="B38" s="4">
         <v>55</v>
       </c>
+      <c r="C38">
+        <v>328.15</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>88</v>
       </c>
@@ -57368,6 +57480,9 @@
       <c r="B39" s="4">
         <v>61</v>
       </c>
+      <c r="C39">
+        <v>334.15</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>89</v>
       </c>
@@ -57380,6 +57495,9 @@
         <f>MEDIAN(80,83)</f>
         <v>81.5</v>
       </c>
+      <c r="C40">
+        <v>354.65</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>90</v>
       </c>
@@ -57391,6 +57509,9 @@
       <c r="B41" s="4">
         <v>61</v>
       </c>
+      <c r="C41">
+        <v>334.15</v>
+      </c>
       <c r="E41" s="1" t="s">
         <v>91</v>
       </c>
@@ -57402,6 +57523,9 @@
       <c r="B42" s="4">
         <v>61</v>
       </c>
+      <c r="C42">
+        <v>334.15</v>
+      </c>
       <c r="E42" s="1" t="s">
         <v>92</v>
       </c>
@@ -57413,6 +57537,9 @@
       <c r="B43" s="4">
         <v>61</v>
       </c>
+      <c r="C43">
+        <v>334.15</v>
+      </c>
       <c r="E43" s="1" t="s">
         <v>93</v>
       </c>
@@ -57424,6 +57551,9 @@
       <c r="B44" s="4">
         <v>61</v>
       </c>
+      <c r="C44">
+        <v>334.15</v>
+      </c>
       <c r="E44" s="1" t="s">
         <v>94</v>
       </c>
@@ -57435,6 +57565,9 @@
       <c r="B45" s="4">
         <v>61</v>
       </c>
+      <c r="C45">
+        <v>334.15</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>95</v>
       </c>
@@ -57446,6 +57579,9 @@
       <c r="B46" s="4">
         <v>61</v>
       </c>
+      <c r="C46">
+        <v>334.15</v>
+      </c>
       <c r="E46" s="1" t="s">
         <v>96</v>
       </c>
@@ -57457,6 +57593,9 @@
       <c r="B47" s="4">
         <v>76</v>
       </c>
+      <c r="C47">
+        <v>349.15</v>
+      </c>
       <c r="E47" s="1" t="s">
         <v>97</v>
       </c>
@@ -57469,6 +57608,9 @@
         <f>MEDIAN(85.5, 86.5)</f>
         <v>86</v>
       </c>
+      <c r="C48">
+        <v>359.15</v>
+      </c>
       <c r="E48" s="1" t="s">
         <v>98</v>
       </c>
@@ -57481,6 +57623,9 @@
         <f>MEDIAN(48, 50)</f>
         <v>49</v>
       </c>
+      <c r="C49">
+        <v>322.14999999999998</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>99</v>
       </c>
@@ -57492,6 +57637,9 @@
       <c r="B50" s="4">
         <v>61</v>
       </c>
+      <c r="C50">
+        <v>334.15</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>100</v>
       </c>
@@ -57503,6 +57651,9 @@
       <c r="B51" s="4">
         <v>61</v>
       </c>
+      <c r="C51">
+        <v>334.15</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>101</v>
       </c>
@@ -57515,6 +57666,9 @@
         <f>MEDIAN(148, 151)</f>
         <v>149.5</v>
       </c>
+      <c r="C52">
+        <v>422.65</v>
+      </c>
       <c r="E52" s="1" t="s">
         <v>102</v>
       </c>
@@ -57526,6 +57680,9 @@
       <c r="B53" s="4">
         <v>222</v>
       </c>
+      <c r="C53">
+        <v>495.15</v>
+      </c>
       <c r="E53" s="1" t="s">
         <v>103</v>
       </c>
@@ -57537,6 +57694,9 @@
       <c r="B54" s="4">
         <v>55</v>
       </c>
+      <c r="C54">
+        <v>328.15</v>
+      </c>
       <c r="E54" s="1" t="s">
         <v>104</v>
       </c>
@@ -57548,6 +57708,9 @@
       <c r="B55" s="4">
         <v>61</v>
       </c>
+      <c r="C55">
+        <v>334.15</v>
+      </c>
       <c r="E55" s="1" t="s">
         <v>105</v>
       </c>
@@ -57559,6 +57722,9 @@
       <c r="B56" s="4">
         <v>55</v>
       </c>
+      <c r="C56">
+        <v>328.15</v>
+      </c>
       <c r="E56" s="1" t="s">
         <v>106</v>
       </c>
@@ -57570,6 +57736,9 @@
       <c r="B57" s="4">
         <v>61</v>
       </c>
+      <c r="C57">
+        <v>334.15</v>
+      </c>
       <c r="E57" s="1" t="s">
         <v>107</v>
       </c>
@@ -57581,6 +57750,9 @@
       <c r="B58" s="4">
         <v>118.68</v>
       </c>
+      <c r="C58">
+        <v>391.83</v>
+      </c>
       <c r="E58" s="1" t="s">
         <v>108</v>
       </c>
@@ -57592,6 +57764,9 @@
       <c r="B59" s="4">
         <v>54</v>
       </c>
+      <c r="C59">
+        <v>327.14999999999998</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>109</v>
       </c>
@@ -57604,6 +57779,9 @@
         <f>MEDIAN(153, 156)</f>
         <v>154.5</v>
       </c>
+      <c r="C60">
+        <v>427.65</v>
+      </c>
       <c r="E60" s="1" t="s">
         <v>110</v>
       </c>
@@ -57615,6 +57793,9 @@
       <c r="B61" s="4">
         <v>61</v>
       </c>
+      <c r="C61">
+        <v>334.15</v>
+      </c>
       <c r="E61" s="1" t="s">
         <v>111</v>
       </c>
@@ -57627,6 +57808,9 @@
         <f>MEDIAN(192,194)</f>
         <v>193</v>
       </c>
+      <c r="C62">
+        <v>466.15</v>
+      </c>
       <c r="E62" s="1" t="s">
         <v>112</v>
       </c>
@@ -57638,6 +57822,9 @@
       <c r="B63" s="4">
         <v>61</v>
       </c>
+      <c r="C63">
+        <v>334.15</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>113</v>
       </c>
@@ -57649,6 +57836,9 @@
       <c r="B64" s="4">
         <v>61</v>
       </c>
+      <c r="C64">
+        <v>334.15</v>
+      </c>
       <c r="E64" s="1" t="s">
         <v>114</v>
       </c>
@@ -57660,6 +57850,9 @@
       <c r="B65" s="4">
         <v>61</v>
       </c>
+      <c r="C65">
+        <v>334.15</v>
+      </c>
       <c r="E65" s="1" t="s">
         <v>115</v>
       </c>
@@ -57671,6 +57864,9 @@
       <c r="B66" s="4">
         <v>61</v>
       </c>
+      <c r="C66">
+        <v>334.15</v>
+      </c>
       <c r="E66" s="1" t="s">
         <v>116</v>
       </c>
@@ -57682,6 +57878,9 @@
       <c r="B67" s="4">
         <v>61</v>
       </c>
+      <c r="C67">
+        <v>334.15</v>
+      </c>
       <c r="E67" s="1" t="s">
         <v>117</v>
       </c>
@@ -57693,6 +57892,9 @@
       <c r="B68" s="4">
         <v>139</v>
       </c>
+      <c r="C68">
+        <v>412.15</v>
+      </c>
       <c r="E68" s="1" t="s">
         <v>118</v>
       </c>
@@ -57704,6 +57906,9 @@
       <c r="B69" s="4">
         <v>350</v>
       </c>
+      <c r="C69">
+        <v>623.15</v>
+      </c>
       <c r="E69" s="1" t="s">
         <v>119</v>
       </c>
@@ -57715,6 +57920,9 @@
       <c r="B70" s="4">
         <v>285</v>
       </c>
+      <c r="C70">
+        <v>558.15</v>
+      </c>
       <c r="E70" s="1" t="s">
         <v>120</v>
       </c>
@@ -57726,6 +57934,9 @@
       <c r="B71" s="4">
         <v>13.8</v>
       </c>
+      <c r="C71">
+        <v>286.95</v>
+      </c>
       <c r="E71" s="1" t="s">
         <v>121</v>
       </c>
@@ -57738,6 +57949,9 @@
         <f>MEDIAN(269,283)</f>
         <v>276</v>
       </c>
+      <c r="C72">
+        <v>549.15</v>
+      </c>
       <c r="E72" s="1" t="s">
         <v>122</v>
       </c>
@@ -57749,6 +57963,9 @@
       <c r="B73" s="4">
         <v>232</v>
       </c>
+      <c r="C73">
+        <v>505.15</v>
+      </c>
       <c r="E73" s="1" t="s">
         <v>123</v>
       </c>
@@ -57761,6 +57978,9 @@
         <f>MEDIAN(244, 247)</f>
         <v>245.5</v>
       </c>
+      <c r="C74">
+        <v>518.65</v>
+      </c>
       <c r="E74" s="1" t="s">
         <v>124</v>
       </c>
@@ -57772,6 +57992,9 @@
       <c r="B75" s="4">
         <v>224</v>
       </c>
+      <c r="C75">
+        <v>497.15</v>
+      </c>
       <c r="E75" s="1" t="s">
         <v>125</v>
       </c>
@@ -57783,6 +58006,9 @@
       <c r="B76" s="4">
         <v>244</v>
       </c>
+      <c r="C76">
+        <v>517.15</v>
+      </c>
       <c r="E76" s="1" t="s">
         <v>126</v>
       </c>
@@ -57794,6 +58020,9 @@
       <c r="B77" s="4">
         <v>190</v>
       </c>
+      <c r="C77">
+        <v>463.15</v>
+      </c>
       <c r="E77" s="1" t="s">
         <v>127</v>
       </c>
@@ -57805,6 +58034,9 @@
       <c r="B78" s="4">
         <v>29</v>
       </c>
+      <c r="C78">
+        <v>302.14999999999998</v>
+      </c>
       <c r="E78" s="1" t="s">
         <v>128</v>
       </c>
@@ -57816,6 +58048,9 @@
       <c r="B79" s="4">
         <v>270</v>
       </c>
+      <c r="C79">
+        <v>543.15</v>
+      </c>
       <c r="E79" s="1" t="s">
         <v>129</v>
       </c>
@@ -57827,6 +58062,9 @@
       <c r="B80" s="4">
         <v>140</v>
       </c>
+      <c r="C80">
+        <v>413.15</v>
+      </c>
       <c r="E80" s="1" t="s">
         <v>130</v>
       </c>
@@ -57838,6 +58076,9 @@
       <c r="B81" s="4">
         <v>185</v>
       </c>
+      <c r="C81">
+        <v>458.15</v>
+      </c>
       <c r="E81" s="1" t="s">
         <v>131</v>
       </c>
@@ -57850,6 +58091,9 @@
         <f>MEDIAN(178, 185)</f>
         <v>181.5</v>
       </c>
+      <c r="C82">
+        <v>454.65</v>
+      </c>
       <c r="E82" s="1" t="s">
         <v>132</v>
       </c>
@@ -57861,6 +58105,9 @@
       <c r="B83" s="4">
         <v>-11.3</v>
       </c>
+      <c r="C83">
+        <v>261.85000000000002</v>
+      </c>
       <c r="E83" s="1" t="s">
         <v>133</v>
       </c>
@@ -57873,6 +58120,9 @@
         <f>MEDIAN(220, 250)</f>
         <v>235</v>
       </c>
+      <c r="C84">
+        <v>508.15</v>
+      </c>
       <c r="E84" s="1" t="s">
         <v>134</v>
       </c>
@@ -57884,6 +58134,9 @@
       <c r="B85" s="4">
         <v>281</v>
       </c>
+      <c r="C85">
+        <v>554.15</v>
+      </c>
       <c r="E85" s="1" t="s">
         <v>135</v>
       </c>
@@ -57895,6 +58148,9 @@
       <c r="B86" s="4">
         <v>268</v>
       </c>
+      <c r="C86">
+        <v>541.15</v>
+      </c>
       <c r="E86" s="1" t="s">
         <v>136</v>
       </c>
@@ -57906,6 +58162,9 @@
       <c r="B87" s="4">
         <v>115</v>
       </c>
+      <c r="C87">
+        <v>388.15</v>
+      </c>
       <c r="E87" s="1" t="s">
         <v>137</v>
       </c>
@@ -57917,6 +58176,9 @@
       <c r="B88" s="4">
         <v>190</v>
       </c>
+      <c r="C88">
+        <v>463.15</v>
+      </c>
       <c r="E88" s="1" t="s">
         <v>138</v>
       </c>
@@ -57928,6 +58190,9 @@
       <c r="B89" s="4">
         <v>247</v>
       </c>
+      <c r="C89">
+        <v>520.15</v>
+      </c>
       <c r="E89" s="1" t="s">
         <v>139</v>
       </c>
@@ -57939,6 +58204,9 @@
       <c r="B90" s="4">
         <v>184</v>
       </c>
+      <c r="C90">
+        <v>457.15</v>
+      </c>
       <c r="E90" s="1" t="s">
         <v>140</v>
       </c>
@@ -57950,6 +58218,9 @@
       <c r="B91" s="4">
         <v>280</v>
       </c>
+      <c r="C91">
+        <v>553.15</v>
+      </c>
       <c r="E91" s="1" t="s">
         <v>141</v>
       </c>
@@ -57961,6 +58232,9 @@
       <c r="B92" s="4">
         <v>211</v>
       </c>
+      <c r="C92">
+        <v>484.15</v>
+      </c>
       <c r="E92" s="1" t="s">
         <v>142</v>
       </c>
@@ -57972,6 +58246,9 @@
       <c r="B93" s="4">
         <v>199</v>
       </c>
+      <c r="C93">
+        <v>472.15</v>
+      </c>
       <c r="E93" s="1" t="s">
         <v>143</v>
       </c>
@@ -57983,6 +58260,9 @@
       <c r="B94" s="4">
         <v>195</v>
       </c>
+      <c r="C94">
+        <v>468.15</v>
+      </c>
       <c r="E94" s="1" t="s">
         <v>144</v>
       </c>
@@ -57994,6 +58274,9 @@
       <c r="B95" s="4">
         <v>233</v>
       </c>
+      <c r="C95">
+        <v>506.15</v>
+      </c>
       <c r="E95" s="1" t="s">
         <v>145</v>
       </c>
@@ -58005,6 +58288,9 @@
       <c r="B96" s="4">
         <v>139</v>
       </c>
+      <c r="C96">
+        <v>412.15</v>
+      </c>
       <c r="E96" s="1" t="s">
         <v>146</v>
       </c>
@@ -58016,6 +58302,9 @@
       <c r="B97" s="4">
         <v>255</v>
       </c>
+      <c r="C97">
+        <v>528.15</v>
+      </c>
       <c r="E97" s="1" t="s">
         <v>147</v>
       </c>
@@ -58027,6 +58316,9 @@
       <c r="B98" s="4">
         <v>286</v>
       </c>
+      <c r="C98">
+        <v>559.15</v>
+      </c>
       <c r="E98" s="1" t="s">
         <v>148</v>
       </c>
@@ -58038,6 +58330,9 @@
       <c r="B99" s="4">
         <v>290</v>
       </c>
+      <c r="C99">
+        <v>563.15</v>
+      </c>
       <c r="E99" s="1" t="s">
         <v>149</v>
       </c>
@@ -58048,6 +58343,9 @@
       </c>
       <c r="B100" s="4">
         <v>240</v>
+      </c>
+      <c r="C100">
+        <v>513.15</v>
       </c>
       <c r="E100" s="1" t="s">
         <v>150</v>
@@ -65532,7 +65830,7 @@
     <mergeCell ref="I1:J3"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -65541,6 +65839,16 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updating and creating xlsx files
</commit_message>
<xml_diff>
--- a/Machine learning/docs/Pubchem_melting_dataset_fromXML.xlsx
+++ b/Machine learning/docs/Pubchem_melting_dataset_fromXML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\BIOINFORMAICS\Machine Learning\Machine learning\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7EFF0C-D7BB-4505-9A1C-BF77BF1891E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58557EDC-12C7-4285-BB79-804C724B72F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{824F0F9F-75C4-40E3-AD7C-0727C9042DB4}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8154" uniqueCount="2529">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8254" uniqueCount="2575">
   <si>
     <t>ns1:SourceName</t>
   </si>
@@ -7631,6 +7631,144 @@
   </si>
   <si>
     <t>max. point [°C] = 350.00 (Cyanocobalamin)</t>
+  </si>
+  <si>
+    <t>CC(=O)Oc1ccccc1C(O)=O</t>
+  </si>
+  <si>
+    <t>CC[C@H](C)[C@H](NC(=O)[C@H](CS)NC(=O)[C@H](CCCCN)NC(=O)[C@H](CC(N)=O)NC(=O)CNC(=O)[C@H](CCC(N)=O)NC(=O)CNC(=O)[C@H](CS)NC(=O)[C@@H](NC(=O)[C@H](CC(N)=O)NC(=O)[C@H](CO)NC(=O)CNC(=O)[C@H](CCC(O)=O)NC(=O)[C@H](CS)NC(=O)[C@H](CC(C)C)NC(=O)[C@H](CS)NC(=O)[C@H](CC(C)C)NC(=O)[C@H](CC(N)=O)NC(=O)[C@H](CCC(N)=O)NC(=O)CNC(=O)[C@H](CO)NC(=O)[C@H](CCC(O)=O)NC(=O)[C@@H](NC(=O)[C@H](CS)NC(=O)[C@H](CC(O)=O)NC(=O)[C@@H](NC(=O)[C@H](Cc1ccc(O)cc1)NC(=O)[C@@H](NC(=O)[C@@H](N)CC(C)C)[C@@H](C)O)[C@@H](C)O)[C@@H](C)O)C(C)C)C(=O)N[C@@H](CC(C)C)C(=O)NCC(=O)N[C@@H](CO)C(=O)N[C@@H](CC(O)=O)C(=O)NCC(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](CCCCN)C(=O)N[C@@H](CC(N)=O)C(=O)N[C@@H](CCC(N)=O)C(=O)N[C@@H](CS)C(=O)N[C@@H](C(C)C)C(=O)N[C@@H]([C@@H](C)O)C(=O)NCC(=O)N[C@@H](CCC(O)=O)C(=O)NCC(=O)N[C@@H]([C@@H](C)O)C(=O)N2CCC[C@H]2C(=O)N[C@@H](CCCCN)C(=O)N3CCC[C@H]3C(=O)N[C@@H](CCC(N)=O)C(=O)N[C@@H](CO)C(=O)N[C@@H](Cc4[nH]cnc4)C(=O)N[C@@H](CC(N)=O)C(=O)N[C@@H](CC(O)=O)C(=O)NCC(=O)N[C@@H](CC(O)=O)C(=O)N[C@@H](Cc5ccccc5)C(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H]([C@@H](C)CC)C(=O)N6CCC[C@H]6C(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](Cc7ccc(O)cc7)C(=O)N[C@@H](CC(C)C)C(=O)N[C@@H](CCC(N)=O)C(O)=O</t>
+  </si>
+  <si>
+    <t>nan</t>
+  </si>
+  <si>
+    <t>CCNC(=O)C1CCCN1C(=O)C(CCCN=C(N)N)NC(=O)C(CC(C)C)NC(=O)C(CC(C)C)NC(=O)C(Cc2ccc(O)cc2)NC(=O)C(CO)NC(=O)C(Cc3c[nH]c4ccccc34)NC(=O)C(Cc5[nH]cnc5)NC(=O)C6CCC(=O)N6</t>
+  </si>
+  <si>
+    <t>CC(C)C[C@@H](NC(=O)[C@H](C)NC(=O)CNC(=O)[C@@H](NC=O)C(C)C)C(=O)N[C@@H](C)C(=O)N[C@H](C(C)C)C(=O)N[C@@H](C(C)C)C(=O)N[C@@H](C(C)C)C(=O)N[C@@H](Cc1c[nH]c2ccccc12)C(=O)N[C@H](CC(C)C)C(=O)N[C@@H](Cc3c[nH]c4ccccc34)C(=O)N[C@H](CC(C)C)C(=O)N[C@@H](Cc5c[nH]c6ccccc56)C(=O)N[C@H](CC(C)C)C(=O)N[C@@H](Cc7c[nH]c8ccccc78)C(=O)NCCO</t>
+  </si>
+  <si>
+    <t>CC[C@H](C)[C@H](NC(=O)CN)C(=O)N[C@@H](C(C)C)C(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](CCC(N)=O)C(=O)N[C@H]1CSSC[C@@H]2NC(=O)[C@@H](NC(=O)[C@H](CO)NC(=O)[C@@H](NC(=O)[C@H](CSSC[C@H](NC(=O)[C@H](CC(C)C)NC(=O)[C@H](Cc3[nH]cnc3)NC(=O)[C@H](CCC(N)=O)NC(=O)[C@H](CC(N)=O)NC(=O)[C@@H](NC(=O)[C@@H](N)Cc4ccccc4)C(C)C)C(=O)NCC(=O)N[C@@H](CO)C(=O)N[C@@H](Cc5[nH]cnc5)C(=O)N[C@@H](CC(C)C)C(=O)N[C@@H](C(C)C)C(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](C)C(=O)N[C@@H](CC(C)C)C(=O)N[C@@H](Cc6ccc(O)cc6)C(=O)N[C@@H](CC(C)C)C(=O)N[C@@H](C(C)C)C(=O)N[C@@H](CSSC[C@H](NC(=O)[C@H](Cc7ccc(O)cc7)NC(=O)[C@H](CC(N)=O)NC(=O)[C@H](CCC(O)=O)NC(=O)[C@H](CC(C)C)NC(=O)[C@H](CCC(N)=O)NC(=O)[C@H](Cc8ccc(O)cc8)NC(=O)[C@H](CC(C)C)NC(=O)[C@H](CO)NC2=O)C(=O)N[C@@H](CC(N)=O)C(O)=O)C(=O)NCC(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](CCCNC(N)=N)C(=O)NCC(=O)N[C@@H](Cc9ccccc9)C(=O)N[C@@H](Cc%10ccccc%10)C(=O)N[C@@H](Cc%11ccc(O)cc%11)C(=O)N[C@@H]([C@@H](C)O)C(=O)N%12CCC[C@H]%12C(=O)N[C@@H](CCCCN)C(=O)N[C@@H]([C@@H](C)O)C(O)=O)NC1=O)[C@@H](C)O)[C@@H](C)CC</t>
+  </si>
+  <si>
+    <t>CC[C@H](C)[C@H](NC(=O)CN)C(=O)N[C@@H](C(C)C)C(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](CCC(N)=O)C(=O)N[C@@H](CS)C(=O)N[C@@H](CS)C(=O)N[C@@H]([C@@H](C)O)C(=O)N[C@@H](CO)C(=O)N[C@@H]([C@@H](C)CC)C(=O)N[C@@H](CS)C(=O)N[C@@H](CO)C(=O)N[C@@H](CC(C)C)C(=O)N[C@@H](Cc1ccc(O)cc1)C(=O)N[C@@H](CCC(N)=O)C(=O)N[C@@H](CC(C)C)C(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](CC(N)=O)C(=O)N[C@@H](Cc2ccc(O)cc2)C(=O)N[C@@H](CS)C(=O)N[C@@H](CC(N)=O)C(O)=O.CC(C)C[C@H](NC(=O)[C@H](C)NC(=O)[C@H](CCC(O)=O)NC(=O)[C@@H](NC(=O)[C@H](CC(C)C)NC(=O)[C@H](Cc3[nH]cnc3)NC(=O)[C@H](CO)NC(=O)CNC(=O)[C@H](CS)NC(=O)[C@H](CC(C)C)NC(=O)[C@H](Cc4[nH]cnc4)NC(=O)[C@H](CCC(N)=O)NC(=O)[C@H](CC(N)=O)NC(=O)[C@@H](NC(=O)[C@@H](N)Cc5ccccc5)C(C)C)C(C)C)C(=O)N[C@@H](Cc6ccc(O)cc6)C(=O)N[C@@H](CC(C)C)C(=O)N[C@@H](C(C)C)C(=O)N[C@@H](CS)C(=O)NCC(=O)N[C@@H](CCC(O)=O)C(=O)N[C@@H](CCCNC(N)=N)C(=O)NCC(=O)N[C@@H](Cc7ccccc7)C(=O)N[C@@H](Cc8ccccc8)C(=O)N[C@@H](Cc9ccc(O)cc9)C(=O)N[C@@H]([C@@H](C)O)C(=O)N[C@@H](CCCCN)C(=O)N%10CCC[C@H]%10C(=O)N[C@@H]([C@@H](C)O)C(O)=O</t>
+  </si>
+  <si>
+    <t>CCC1NC(=O)C(C(O)C(C)C\C=C\C)N(C)C(=O)C(C(C)C)N(C)C(=O)C(CC(C)C)N(C)C(=O)C(CC(C)C)N(C)C(=O)C(C)NC(=O)C(C)NC(=O)C(CC(C)C)N(C)C(=O)C(NC(=O)C(CC(C)C)N(C)C(=O)CN(C)C1=O)C(C)C</t>
+  </si>
+  <si>
+    <t>NCCCCC(NC(=O)C1CCCN1C(=O)C2CSSCC(N)C(=O)NC(Cc3ccccc3)C(=O)NC(Cc4ccccc4)C(=O)NC(CCC(N)=O)C(=O)NC(CC(N)=O)C(=O)N2)C(=O)NCC(N)=O</t>
+  </si>
+  <si>
+    <t>CCC(C)C1NC(=O)C(Cc2ccc(O)cc2)NC(=O)C(N)CSSCC(NC(=O)C(CC(N)=O)NC(=O)C(NC1=O)C(C)O)C(=O)N3CCCC3C(=O)NC(CC(C)C)C(=O)NCC(N)=O</t>
+  </si>
+  <si>
+    <t>CC(O)C(CO)NC(=O)C1CSSCC(NC(=O)C(N)Cc2ccccc2)C(=O)NC(Cc3ccccc3)C(=O)NC(Cc4c[nH]c5ccccc45)C(=O)NC(CCCCN)C(=O)NC(C(C)O)C(=O)N1</t>
+  </si>
+  <si>
+    <t>CC[C@H](C)[C@@H]1NC(=O)[C@H](Cc2ccc(O)cc2)NC(=O)[C@@H](N)CSSC[C@H](NC(=O)[C@H](CC(N)=O)NC(=O)[C@H](CCC(N)=O)NC1=O)C(=O)N3CCC[C@H]3C(=O)N[C@@H](CC(C)C)C(=O)NCC(N)=O</t>
+  </si>
+  <si>
+    <t>O.Cc1ncc(CO[P](O)(O)=O)c(C=O)c1O</t>
+  </si>
+  <si>
+    <t>[Co+3]|[C-]#N.C[C@H](CNC(=O)CC[C@]1(C)[C@@H](CC(N)=O)[C@H]2N=C1C(=C3[N-]C(=CC4=NC(=C(C)C5=N[C@]2(C)[C@@](C)(CC(N)=O)[C@@H]5CCC(N)=O)[C@@](C)(CC(N)=O)[C@@H]4CCC(N)=O)C(C)(C)[C@@H]3CCC(N)=O)C)O[P]([O-])(=O)O[C@H]6[C@@H](O)[C@H](O[C@@H]6CO)n7cnc8cc(C)c(C)cc78</t>
+  </si>
+  <si>
+    <t>N[C@@H](Cc1c[nH]cn1)C(O)=O</t>
+  </si>
+  <si>
+    <t>CC(=O)C(O)=O</t>
+  </si>
+  <si>
+    <t>N[C@@H](Cc1ccccc1)C(O)=O</t>
+  </si>
+  <si>
+    <t>OC(=O)CCCCC1SCC2NC(=O)NC12</t>
+  </si>
+  <si>
+    <t>C[N+](C)(C)CCO</t>
+  </si>
+  <si>
+    <t>NCCCC[C@H](N)C(O)=O</t>
+  </si>
+  <si>
+    <t>N[C@@H](CCCNC(N)=N)C(O)=O</t>
+  </si>
+  <si>
+    <t>OCC(O)C1OC(=C(O)C1=O)O</t>
+  </si>
+  <si>
+    <t>NCCCNCCCCNCCCN</t>
+  </si>
+  <si>
+    <t>N[C@@H](CC(O)=O)C(O)=O</t>
+  </si>
+  <si>
+    <t>NCCC[C@H](N)C(O)=O</t>
+  </si>
+  <si>
+    <t>N[C@@H](CCC(N)=O)C(O)=O</t>
+  </si>
+  <si>
+    <t>Nc1ncnc2n(cnc12)[C@@H]3O[C@H](CO[P](O)(O)=O)[C@@H](O)[C@H]3O</t>
+  </si>
+  <si>
+    <t>CC\C=C/C/C=C\C\C=C/CCCCCCCC(O)=O</t>
+  </si>
+  <si>
+    <t>N[C@@H](CO)C(O)=O</t>
+  </si>
+  <si>
+    <t>CSCC[C@H](N)C(O)=O</t>
+  </si>
+  <si>
+    <t>N[C@@H](Cc1ccc(O)cc1)C(O)=O</t>
+  </si>
+  <si>
+    <t>C[C@H](CCCC(C)(C)O)[C@H]1CC[C@H]2\C(CCC[C@]12C)=C\C=C3\C[C@@H](O)C[C@H](O)C3=C</t>
+  </si>
+  <si>
+    <t>CC(=C\C=C\C=C(C)\C=C\C=C(C)\C=C\C1=C(C)C[C@@H](O)CC1(C)C)/C=C/C=C(C)/C=C/[C@H]2C(=C[C@H](O)CC2(C)C)C</t>
+  </si>
+  <si>
+    <t>N[C@@H](CSSC[C@H](N)C(O)=O)C(O)=O</t>
+  </si>
+  <si>
+    <t>OC(=O)CCC(O)=O</t>
+  </si>
+  <si>
+    <t>Cc1cc2N=C3C(=O)NC(=O)N=C3N(CC(O)C(O)C(O)CO)c2cc1C</t>
+  </si>
+  <si>
+    <t>CC(=O)N[C@H]1C(O)O[C@H](CO)[C@@H](O)[C@@H]1O</t>
+  </si>
+  <si>
+    <t>N[C@@H](CCC(O)=O)C(O)=O</t>
+  </si>
+  <si>
+    <t>N[C@@H](CCC(=O)N[C@@H](CS)C(=O)NCC(O)=O)C(O)=O</t>
+  </si>
+  <si>
+    <t>NCC(O)=O</t>
+  </si>
+  <si>
+    <t>Cc1ncc(CO)c(C=O)c1O</t>
+  </si>
+  <si>
+    <t>CN(CC(O)=O)C(N)=N</t>
+  </si>
+  <si>
+    <t>CC(C)C[C@H](N)C(O)=O</t>
+  </si>
+  <si>
+    <t>N[C@@H](Cc1c[nH]c2ccccc12)C(O)=O</t>
+  </si>
+  <si>
+    <t>N[C@@H](CS)C(O)=O</t>
+  </si>
+  <si>
+    <t>[Cl-].Cc1ncc(C[n+]2csc(CCO)c2C)c(N)n1</t>
   </si>
 </sst>
 </file>
@@ -56897,7 +57035,7 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -56905,7 +57043,7 @@
     <col min="1" max="1" width="38.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="4" customWidth="1"/>
     <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="38.5546875" customWidth="1"/>
     <col min="5" max="5" width="11.5546875" customWidth="1"/>
     <col min="9" max="9" width="33.44140625" customWidth="1"/>
     <col min="10" max="10" width="29.6640625" customWidth="1"/>
@@ -56942,6 +57080,9 @@
       <c r="C2">
         <v>408.15</v>
       </c>
+      <c r="D2" t="s">
+        <v>2529</v>
+      </c>
       <c r="E2" s="1" t="s">
         <v>52</v>
       </c>
@@ -56958,6 +57099,9 @@
       <c r="C3">
         <v>331.15</v>
       </c>
+      <c r="D3" t="s">
+        <v>2530</v>
+      </c>
       <c r="E3" s="1" t="s">
         <v>53</v>
       </c>
@@ -56974,6 +57118,9 @@
       <c r="C4">
         <v>334.15</v>
       </c>
+      <c r="D4" t="s">
+        <v>2531</v>
+      </c>
       <c r="E4" s="1" t="s">
         <v>54</v>
       </c>
@@ -56992,6 +57139,9 @@
       <c r="C5">
         <v>340.15</v>
       </c>
+      <c r="D5" t="s">
+        <v>2531</v>
+      </c>
       <c r="E5" s="1" t="s">
         <v>55</v>
       </c>
@@ -57008,6 +57158,9 @@
       <c r="C6">
         <v>344.15</v>
       </c>
+      <c r="D6" t="s">
+        <v>2531</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>56</v>
       </c>
@@ -57027,6 +57180,9 @@
       <c r="C7">
         <v>425.65</v>
       </c>
+      <c r="D7" t="s">
+        <v>2532</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>57</v>
       </c>
@@ -57044,6 +57200,9 @@
       <c r="C8">
         <v>330.55</v>
       </c>
+      <c r="D8" t="s">
+        <v>2531</v>
+      </c>
       <c r="E8" s="1" t="s">
         <v>58</v>
       </c>
@@ -57058,6 +57217,9 @@
       <c r="C9">
         <v>333.15</v>
       </c>
+      <c r="D9" t="s">
+        <v>2531</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>59</v>
       </c>
@@ -57072,6 +57234,9 @@
       <c r="C10">
         <v>334.15</v>
       </c>
+      <c r="D10" t="s">
+        <v>2531</v>
+      </c>
       <c r="E10" s="1" t="s">
         <v>60</v>
       </c>
@@ -57086,6 +57251,9 @@
       <c r="C11">
         <v>326.14999999999998</v>
       </c>
+      <c r="D11" t="s">
+        <v>2531</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>61</v>
       </c>
@@ -57101,6 +57269,9 @@
       <c r="C12">
         <v>349.15</v>
       </c>
+      <c r="D12" t="s">
+        <v>2531</v>
+      </c>
       <c r="E12" s="1" t="s">
         <v>62</v>
       </c>
@@ -57115,6 +57286,9 @@
       <c r="C13">
         <v>333.15</v>
       </c>
+      <c r="D13" t="s">
+        <v>2531</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>63</v>
       </c>
@@ -57129,6 +57303,9 @@
       <c r="C14">
         <v>326.14999999999998</v>
       </c>
+      <c r="D14" t="s">
+        <v>2531</v>
+      </c>
       <c r="E14" s="1" t="s">
         <v>64</v>
       </c>
@@ -57143,6 +57320,9 @@
       <c r="C15">
         <v>334.15</v>
       </c>
+      <c r="D15" t="s">
+        <v>2531</v>
+      </c>
       <c r="E15" s="1" t="s">
         <v>65</v>
       </c>
@@ -57158,6 +57338,9 @@
       <c r="C16">
         <v>278.14999999999998</v>
       </c>
+      <c r="D16" t="s">
+        <v>2531</v>
+      </c>
       <c r="E16" s="1" t="s">
         <v>66</v>
       </c>
@@ -57172,6 +57355,9 @@
       <c r="C17">
         <v>330.15</v>
       </c>
+      <c r="D17" t="s">
+        <v>2531</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>67</v>
       </c>
@@ -57186,6 +57372,9 @@
       <c r="C18">
         <v>328.15</v>
       </c>
+      <c r="D18" t="s">
+        <v>2531</v>
+      </c>
       <c r="E18" s="1" t="s">
         <v>68</v>
       </c>
@@ -57201,6 +57390,9 @@
       <c r="C19">
         <v>502.65</v>
       </c>
+      <c r="D19" t="s">
+        <v>2533</v>
+      </c>
       <c r="E19" s="1" t="s">
         <v>69</v>
       </c>
@@ -57215,6 +57407,9 @@
       <c r="C20">
         <v>343.15</v>
       </c>
+      <c r="D20" t="s">
+        <v>2531</v>
+      </c>
       <c r="E20" s="1" t="s">
         <v>70</v>
       </c>
@@ -57229,6 +57424,9 @@
       <c r="C21">
         <v>333.15</v>
       </c>
+      <c r="D21" t="s">
+        <v>2531</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>71</v>
       </c>
@@ -57243,6 +57441,9 @@
       <c r="C22">
         <v>354.15</v>
       </c>
+      <c r="D22" t="s">
+        <v>2534</v>
+      </c>
       <c r="E22" s="1" t="s">
         <v>72</v>
       </c>
@@ -57257,6 +57458,9 @@
       <c r="C23">
         <v>333.15</v>
       </c>
+      <c r="D23" t="s">
+        <v>2531</v>
+      </c>
       <c r="E23" s="1" t="s">
         <v>73</v>
       </c>
@@ -57271,6 +57475,9 @@
       <c r="C24">
         <v>328.15</v>
       </c>
+      <c r="D24" t="s">
+        <v>2531</v>
+      </c>
       <c r="E24" s="1" t="s">
         <v>74</v>
       </c>
@@ -57285,6 +57492,9 @@
       <c r="C25">
         <v>334.15</v>
       </c>
+      <c r="D25" t="s">
+        <v>2531</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>75</v>
       </c>
@@ -57299,6 +57509,9 @@
       <c r="C26">
         <v>331.15</v>
       </c>
+      <c r="D26" t="s">
+        <v>2531</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>76</v>
       </c>
@@ -57313,6 +57526,9 @@
       <c r="C27">
         <v>334.15</v>
       </c>
+      <c r="D27" t="s">
+        <v>2531</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>77</v>
       </c>
@@ -57327,6 +57543,9 @@
       <c r="C28">
         <v>328.15</v>
       </c>
+      <c r="D28" t="s">
+        <v>2531</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>78</v>
       </c>
@@ -57341,6 +57560,9 @@
       <c r="C29">
         <v>354.15</v>
       </c>
+      <c r="D29" t="s">
+        <v>2535</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>79</v>
       </c>
@@ -57355,6 +57577,9 @@
       <c r="C30">
         <v>354.15</v>
       </c>
+      <c r="D30" t="s">
+        <v>2531</v>
+      </c>
       <c r="E30" s="1" t="s">
         <v>80</v>
       </c>
@@ -57370,6 +57595,9 @@
       <c r="C31">
         <v>324.64999999999998</v>
       </c>
+      <c r="D31" t="s">
+        <v>2531</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>81</v>
       </c>
@@ -57384,6 +57612,9 @@
       <c r="C32">
         <v>349.15</v>
       </c>
+      <c r="D32" t="s">
+        <v>2531</v>
+      </c>
       <c r="E32" s="1" t="s">
         <v>82</v>
       </c>
@@ -57398,6 +57629,9 @@
       <c r="C33">
         <v>334.15</v>
       </c>
+      <c r="D33" t="s">
+        <v>2531</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>83</v>
       </c>
@@ -57412,6 +57646,9 @@
       <c r="C34">
         <v>334.15</v>
       </c>
+      <c r="D34" t="s">
+        <v>2531</v>
+      </c>
       <c r="E34" s="1" t="s">
         <v>84</v>
       </c>
@@ -57426,6 +57663,9 @@
       <c r="C35">
         <v>334.15</v>
       </c>
+      <c r="D35" t="s">
+        <v>2531</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>85</v>
       </c>
@@ -57441,6 +57681,9 @@
       <c r="C36">
         <v>328.15</v>
       </c>
+      <c r="D36" t="s">
+        <v>2531</v>
+      </c>
       <c r="E36" s="1" t="s">
         <v>86</v>
       </c>
@@ -57455,6 +57698,9 @@
       <c r="C37">
         <v>334.15</v>
       </c>
+      <c r="D37" t="s">
+        <v>2531</v>
+      </c>
       <c r="E37" s="1" t="s">
         <v>87</v>
       </c>
@@ -57469,6 +57715,9 @@
       <c r="C38">
         <v>328.15</v>
       </c>
+      <c r="D38" t="s">
+        <v>2531</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>88</v>
       </c>
@@ -57483,6 +57732,9 @@
       <c r="C39">
         <v>334.15</v>
       </c>
+      <c r="D39" t="s">
+        <v>2531</v>
+      </c>
       <c r="E39" s="1" t="s">
         <v>89</v>
       </c>
@@ -57498,6 +57750,9 @@
       <c r="C40">
         <v>354.65</v>
       </c>
+      <c r="D40" t="s">
+        <v>2531</v>
+      </c>
       <c r="E40" s="1" t="s">
         <v>90</v>
       </c>
@@ -57512,6 +57767,9 @@
       <c r="C41">
         <v>334.15</v>
       </c>
+      <c r="D41" t="s">
+        <v>2531</v>
+      </c>
       <c r="E41" s="1" t="s">
         <v>91</v>
       </c>
@@ -57526,6 +57784,9 @@
       <c r="C42">
         <v>334.15</v>
       </c>
+      <c r="D42" t="s">
+        <v>2531</v>
+      </c>
       <c r="E42" s="1" t="s">
         <v>92</v>
       </c>
@@ -57540,6 +57801,9 @@
       <c r="C43">
         <v>334.15</v>
       </c>
+      <c r="D43" t="s">
+        <v>2531</v>
+      </c>
       <c r="E43" s="1" t="s">
         <v>93</v>
       </c>
@@ -57554,6 +57818,9 @@
       <c r="C44">
         <v>334.15</v>
       </c>
+      <c r="D44" t="s">
+        <v>2531</v>
+      </c>
       <c r="E44" s="1" t="s">
         <v>94</v>
       </c>
@@ -57568,6 +57835,9 @@
       <c r="C45">
         <v>334.15</v>
       </c>
+      <c r="D45" t="s">
+        <v>2531</v>
+      </c>
       <c r="E45" s="1" t="s">
         <v>95</v>
       </c>
@@ -57582,6 +57852,9 @@
       <c r="C46">
         <v>334.15</v>
       </c>
+      <c r="D46" t="s">
+        <v>2531</v>
+      </c>
       <c r="E46" s="1" t="s">
         <v>96</v>
       </c>
@@ -57596,6 +57869,9 @@
       <c r="C47">
         <v>349.15</v>
       </c>
+      <c r="D47" t="s">
+        <v>2531</v>
+      </c>
       <c r="E47" s="1" t="s">
         <v>97</v>
       </c>
@@ -57611,6 +57887,9 @@
       <c r="C48">
         <v>359.15</v>
       </c>
+      <c r="D48" t="s">
+        <v>2531</v>
+      </c>
       <c r="E48" s="1" t="s">
         <v>98</v>
       </c>
@@ -57626,6 +57905,9 @@
       <c r="C49">
         <v>322.14999999999998</v>
       </c>
+      <c r="D49" t="s">
+        <v>2531</v>
+      </c>
       <c r="E49" s="1" t="s">
         <v>99</v>
       </c>
@@ -57640,6 +57922,9 @@
       <c r="C50">
         <v>334.15</v>
       </c>
+      <c r="D50" t="s">
+        <v>2531</v>
+      </c>
       <c r="E50" s="1" t="s">
         <v>100</v>
       </c>
@@ -57654,6 +57939,9 @@
       <c r="C51">
         <v>334.15</v>
       </c>
+      <c r="D51" t="s">
+        <v>2531</v>
+      </c>
       <c r="E51" s="1" t="s">
         <v>101</v>
       </c>
@@ -57669,6 +57957,9 @@
       <c r="C52">
         <v>422.65</v>
       </c>
+      <c r="D52" t="s">
+        <v>2536</v>
+      </c>
       <c r="E52" s="1" t="s">
         <v>102</v>
       </c>
@@ -57683,6 +57974,9 @@
       <c r="C53">
         <v>495.15</v>
       </c>
+      <c r="D53" t="s">
+        <v>2537</v>
+      </c>
       <c r="E53" s="1" t="s">
         <v>103</v>
       </c>
@@ -57697,6 +57991,9 @@
       <c r="C54">
         <v>328.15</v>
       </c>
+      <c r="D54" t="s">
+        <v>2538</v>
+      </c>
       <c r="E54" s="1" t="s">
         <v>104</v>
       </c>
@@ -57711,6 +58008,9 @@
       <c r="C55">
         <v>334.15</v>
       </c>
+      <c r="D55" t="s">
+        <v>2531</v>
+      </c>
       <c r="E55" s="1" t="s">
         <v>105</v>
       </c>
@@ -57725,6 +58025,9 @@
       <c r="C56">
         <v>328.15</v>
       </c>
+      <c r="D56" t="s">
+        <v>2531</v>
+      </c>
       <c r="E56" s="1" t="s">
         <v>106</v>
       </c>
@@ -57739,6 +58042,9 @@
       <c r="C57">
         <v>334.15</v>
       </c>
+      <c r="D57" t="s">
+        <v>2531</v>
+      </c>
       <c r="E57" s="1" t="s">
         <v>107</v>
       </c>
@@ -57753,6 +58059,9 @@
       <c r="C58">
         <v>391.83</v>
       </c>
+      <c r="D58" t="s">
+        <v>2531</v>
+      </c>
       <c r="E58" s="1" t="s">
         <v>108</v>
       </c>
@@ -57767,6 +58076,9 @@
       <c r="C59">
         <v>327.14999999999998</v>
       </c>
+      <c r="D59" t="s">
+        <v>2531</v>
+      </c>
       <c r="E59" s="1" t="s">
         <v>109</v>
       </c>
@@ -57782,6 +58094,9 @@
       <c r="C60">
         <v>427.65</v>
       </c>
+      <c r="D60" t="s">
+        <v>2539</v>
+      </c>
       <c r="E60" s="1" t="s">
         <v>110</v>
       </c>
@@ -57796,6 +58111,9 @@
       <c r="C61">
         <v>334.15</v>
       </c>
+      <c r="D61" t="s">
+        <v>2531</v>
+      </c>
       <c r="E61" s="1" t="s">
         <v>111</v>
       </c>
@@ -57811,6 +58129,9 @@
       <c r="C62">
         <v>466.15</v>
       </c>
+      <c r="D62" t="s">
+        <v>2540</v>
+      </c>
       <c r="E62" s="1" t="s">
         <v>112</v>
       </c>
@@ -57825,6 +58146,9 @@
       <c r="C63">
         <v>334.15</v>
       </c>
+      <c r="D63" t="s">
+        <v>2531</v>
+      </c>
       <c r="E63" s="1" t="s">
         <v>113</v>
       </c>
@@ -57839,6 +58163,9 @@
       <c r="C64">
         <v>334.15</v>
       </c>
+      <c r="D64" t="s">
+        <v>2531</v>
+      </c>
       <c r="E64" s="1" t="s">
         <v>114</v>
       </c>
@@ -57853,6 +58180,9 @@
       <c r="C65">
         <v>334.15</v>
       </c>
+      <c r="D65" t="s">
+        <v>2531</v>
+      </c>
       <c r="E65" s="1" t="s">
         <v>115</v>
       </c>
@@ -57867,6 +58197,9 @@
       <c r="C66">
         <v>334.15</v>
       </c>
+      <c r="D66" t="s">
+        <v>2531</v>
+      </c>
       <c r="E66" s="1" t="s">
         <v>116</v>
       </c>
@@ -57881,6 +58214,9 @@
       <c r="C67">
         <v>334.15</v>
       </c>
+      <c r="D67" t="s">
+        <v>2531</v>
+      </c>
       <c r="E67" s="1" t="s">
         <v>117</v>
       </c>
@@ -57895,6 +58231,9 @@
       <c r="C68">
         <v>412.15</v>
       </c>
+      <c r="D68" t="s">
+        <v>2541</v>
+      </c>
       <c r="E68" s="1" t="s">
         <v>118</v>
       </c>
@@ -57909,6 +58248,9 @@
       <c r="C69">
         <v>623.15</v>
       </c>
+      <c r="D69" t="s">
+        <v>2542</v>
+      </c>
       <c r="E69" s="1" t="s">
         <v>119</v>
       </c>
@@ -57923,6 +58265,9 @@
       <c r="C70">
         <v>558.15</v>
       </c>
+      <c r="D70" t="s">
+        <v>2543</v>
+      </c>
       <c r="E70" s="1" t="s">
         <v>120</v>
       </c>
@@ -57937,6 +58282,9 @@
       <c r="C71">
         <v>286.95</v>
       </c>
+      <c r="D71" t="s">
+        <v>2544</v>
+      </c>
       <c r="E71" s="1" t="s">
         <v>121</v>
       </c>
@@ -57952,6 +58300,9 @@
       <c r="C72">
         <v>549.15</v>
       </c>
+      <c r="D72" t="s">
+        <v>2545</v>
+      </c>
       <c r="E72" s="1" t="s">
         <v>122</v>
       </c>
@@ -57966,6 +58317,9 @@
       <c r="C73">
         <v>505.15</v>
       </c>
+      <c r="D73" t="s">
+        <v>2546</v>
+      </c>
       <c r="E73" s="1" t="s">
         <v>123</v>
       </c>
@@ -57981,6 +58335,9 @@
       <c r="C74">
         <v>518.65</v>
       </c>
+      <c r="D74" t="s">
+        <v>2547</v>
+      </c>
       <c r="E74" s="1" t="s">
         <v>124</v>
       </c>
@@ -57995,6 +58352,9 @@
       <c r="C75">
         <v>497.15</v>
       </c>
+      <c r="D75" t="s">
+        <v>2548</v>
+      </c>
       <c r="E75" s="1" t="s">
         <v>125</v>
       </c>
@@ -58009,6 +58369,9 @@
       <c r="C76">
         <v>517.15</v>
       </c>
+      <c r="D76" t="s">
+        <v>2549</v>
+      </c>
       <c r="E76" s="1" t="s">
         <v>126</v>
       </c>
@@ -58023,6 +58386,9 @@
       <c r="C77">
         <v>463.15</v>
       </c>
+      <c r="D77" t="s">
+        <v>2550</v>
+      </c>
       <c r="E77" s="1" t="s">
         <v>127</v>
       </c>
@@ -58037,6 +58403,9 @@
       <c r="C78">
         <v>302.14999999999998</v>
       </c>
+      <c r="D78" t="s">
+        <v>2551</v>
+      </c>
       <c r="E78" s="1" t="s">
         <v>128</v>
       </c>
@@ -58051,6 +58420,9 @@
       <c r="C79">
         <v>543.15</v>
       </c>
+      <c r="D79" t="s">
+        <v>2552</v>
+      </c>
       <c r="E79" s="1" t="s">
         <v>129</v>
       </c>
@@ -58065,6 +58437,9 @@
       <c r="C80">
         <v>413.15</v>
       </c>
+      <c r="D80" t="s">
+        <v>2553</v>
+      </c>
       <c r="E80" s="1" t="s">
         <v>130</v>
       </c>
@@ -58079,6 +58454,9 @@
       <c r="C81">
         <v>458.15</v>
       </c>
+      <c r="D81" t="s">
+        <v>2554</v>
+      </c>
       <c r="E81" s="1" t="s">
         <v>131</v>
       </c>
@@ -58094,6 +58472,9 @@
       <c r="C82">
         <v>454.65</v>
       </c>
+      <c r="D82" t="s">
+        <v>2555</v>
+      </c>
       <c r="E82" s="1" t="s">
         <v>132</v>
       </c>
@@ -58108,6 +58489,9 @@
       <c r="C83">
         <v>261.85000000000002</v>
       </c>
+      <c r="D83" t="s">
+        <v>2556</v>
+      </c>
       <c r="E83" s="1" t="s">
         <v>133</v>
       </c>
@@ -58123,6 +58507,9 @@
       <c r="C84">
         <v>508.15</v>
       </c>
+      <c r="D84" t="s">
+        <v>2557</v>
+      </c>
       <c r="E84" s="1" t="s">
         <v>134</v>
       </c>
@@ -58137,6 +58524,9 @@
       <c r="C85">
         <v>554.15</v>
       </c>
+      <c r="D85" t="s">
+        <v>2558</v>
+      </c>
       <c r="E85" s="1" t="s">
         <v>135</v>
       </c>
@@ -58151,6 +58541,9 @@
       <c r="C86">
         <v>541.15</v>
       </c>
+      <c r="D86" t="s">
+        <v>2559</v>
+      </c>
       <c r="E86" s="1" t="s">
         <v>136</v>
       </c>
@@ -58165,6 +58558,9 @@
       <c r="C87">
         <v>388.15</v>
       </c>
+      <c r="D87" t="s">
+        <v>2560</v>
+      </c>
       <c r="E87" s="1" t="s">
         <v>137</v>
       </c>
@@ -58179,6 +58575,9 @@
       <c r="C88">
         <v>463.15</v>
       </c>
+      <c r="D88" t="s">
+        <v>2561</v>
+      </c>
       <c r="E88" s="1" t="s">
         <v>138</v>
       </c>
@@ -58193,6 +58592,9 @@
       <c r="C89">
         <v>520.15</v>
       </c>
+      <c r="D89" t="s">
+        <v>2562</v>
+      </c>
       <c r="E89" s="1" t="s">
         <v>139</v>
       </c>
@@ -58207,6 +58609,9 @@
       <c r="C90">
         <v>457.15</v>
       </c>
+      <c r="D90" t="s">
+        <v>2563</v>
+      </c>
       <c r="E90" s="1" t="s">
         <v>140</v>
       </c>
@@ -58221,6 +58626,9 @@
       <c r="C91">
         <v>553.15</v>
       </c>
+      <c r="D91" t="s">
+        <v>2564</v>
+      </c>
       <c r="E91" s="1" t="s">
         <v>141</v>
       </c>
@@ -58235,6 +58643,9 @@
       <c r="C92">
         <v>484.15</v>
       </c>
+      <c r="D92" t="s">
+        <v>2565</v>
+      </c>
       <c r="E92" s="1" t="s">
         <v>142</v>
       </c>
@@ -58249,6 +58660,9 @@
       <c r="C93">
         <v>472.15</v>
       </c>
+      <c r="D93" t="s">
+        <v>2566</v>
+      </c>
       <c r="E93" s="1" t="s">
         <v>143</v>
       </c>
@@ -58263,6 +58677,9 @@
       <c r="C94">
         <v>468.15</v>
       </c>
+      <c r="D94" t="s">
+        <v>2567</v>
+      </c>
       <c r="E94" s="1" t="s">
         <v>144</v>
       </c>
@@ -58277,6 +58694,9 @@
       <c r="C95">
         <v>506.15</v>
       </c>
+      <c r="D95" t="s">
+        <v>2568</v>
+      </c>
       <c r="E95" s="1" t="s">
         <v>145</v>
       </c>
@@ -58291,6 +58711,9 @@
       <c r="C96">
         <v>412.15</v>
       </c>
+      <c r="D96" t="s">
+        <v>2569</v>
+      </c>
       <c r="E96" s="1" t="s">
         <v>146</v>
       </c>
@@ -58305,6 +58728,9 @@
       <c r="C97">
         <v>528.15</v>
       </c>
+      <c r="D97" t="s">
+        <v>2570</v>
+      </c>
       <c r="E97" s="1" t="s">
         <v>147</v>
       </c>
@@ -58319,6 +58745,9 @@
       <c r="C98">
         <v>559.15</v>
       </c>
+      <c r="D98" t="s">
+        <v>2571</v>
+      </c>
       <c r="E98" s="1" t="s">
         <v>148</v>
       </c>
@@ -58333,6 +58762,9 @@
       <c r="C99">
         <v>563.15</v>
       </c>
+      <c r="D99" t="s">
+        <v>2572</v>
+      </c>
       <c r="E99" s="1" t="s">
         <v>149</v>
       </c>
@@ -58347,6 +58779,9 @@
       <c r="C100">
         <v>513.15</v>
       </c>
+      <c r="D100" t="s">
+        <v>2573</v>
+      </c>
       <c r="E100" s="1" t="s">
         <v>150</v>
       </c>
@@ -58354,6 +58789,9 @@
     <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>1151</v>
+      </c>
+      <c r="D101" t="s">
+        <v>2574</v>
       </c>
       <c r="E101" s="1" t="s">
         <v>151</v>

</xml_diff>

<commit_message>
adding bayes kNN and tree algorithms, attending workshop program, starting deep learning algorithms...
</commit_message>
<xml_diff>
--- a/Machine learning/docs/Pubchem_melting_dataset_fromXML.xlsx
+++ b/Machine learning/docs/Pubchem_melting_dataset_fromXML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\BIOINFORMAICS\Machine Learning\Machine learning\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58557EDC-12C7-4285-BB79-804C724B72F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D491C2-0D22-4F9D-8D8C-511419E7202C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{824F0F9F-75C4-40E3-AD7C-0727C9042DB4}"/>
   </bookViews>
@@ -57035,7 +57035,7 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
working with melting point prediction of drugs.
</commit_message>
<xml_diff>
--- a/Machine learning/docs/Pubchem_melting_dataset_fromXML.xlsx
+++ b/Machine learning/docs/Pubchem_melting_dataset_fromXML.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\BIOINFORMAICS\Machine Learning\Machine learning\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58D491C2-0D22-4F9D-8D8C-511419E7202C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEF30A6A-E30E-44F6-9ACC-F88424246B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{824F0F9F-75C4-40E3-AD7C-0727C9042DB4}"/>
   </bookViews>
@@ -57035,7 +57035,7 @@
   <dimension ref="A1:J1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>